<commit_message>
Finished lab report, and updated the chart on the excel doc
</commit_message>
<xml_diff>
--- a/Chart Data.xlsx
+++ b/Chart Data.xlsx
@@ -13017,11 +13017,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="295334928"/>
-        <c:axId val="295321992"/>
+        <c:axId val="469112032"/>
+        <c:axId val="469113208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="295334928"/>
+        <c:axId val="469112032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13041,6 +13041,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time(s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -13078,12 +13134,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295321992"/>
+        <c:crossAx val="469113208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="295321992"/>
+        <c:axId val="469113208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13103,6 +13159,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -13140,7 +13252,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="295334928"/>
+        <c:crossAx val="469112032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -19321,11 +19433,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="293759672"/>
-        <c:axId val="293747912"/>
+        <c:axId val="469115560"/>
+        <c:axId val="469114384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="293759672"/>
+        <c:axId val="469115560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19382,12 +19494,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293747912"/>
+        <c:crossAx val="469114384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="293747912"/>
+        <c:axId val="469114384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19444,7 +19556,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293759672"/>
+        <c:crossAx val="469115560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20640,7 +20752,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -20651,7 +20763,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8676238" cy="6290272"/>
+    <xdr:ext cx="8660876" cy="6294356"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>

</xml_diff>